<commit_message>
updated EI Data with june 2023
</commit_message>
<xml_diff>
--- a/Economic_Indicators_Data/data/transformed_data/bci.xlsx
+++ b/Economic_Indicators_Data/data/transformed_data/bci.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saide\Documents\Final_Year_Dissertation\Economic_Indicators_Data\data\processed_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saide\Documents\Final_Year_Dissertation\Economic_Indicators_Data\data\transformed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F34E1B-3E2C-41E2-8FC7-302B327A2350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603274C-0275-4C93-A468-AF92892F9E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="1828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="2009">
   <si>
     <t>TIME</t>
   </si>
@@ -5504,6 +5504,549 @@
   </si>
   <si>
     <t>31-12-2022</t>
+  </si>
+  <si>
+    <t>01-01-2023</t>
+  </si>
+  <si>
+    <t>02-01-2023</t>
+  </si>
+  <si>
+    <t>03-01-2023</t>
+  </si>
+  <si>
+    <t>04-01-2023</t>
+  </si>
+  <si>
+    <t>05-01-2023</t>
+  </si>
+  <si>
+    <t>06-01-2023</t>
+  </si>
+  <si>
+    <t>07-01-2023</t>
+  </si>
+  <si>
+    <t>08-01-2023</t>
+  </si>
+  <si>
+    <t>09-01-2023</t>
+  </si>
+  <si>
+    <t>10-01-2023</t>
+  </si>
+  <si>
+    <t>11-01-2023</t>
+  </si>
+  <si>
+    <t>12-01-2023</t>
+  </si>
+  <si>
+    <t>13-01-2023</t>
+  </si>
+  <si>
+    <t>14-01-2023</t>
+  </si>
+  <si>
+    <t>15-01-2023</t>
+  </si>
+  <si>
+    <t>16-01-2023</t>
+  </si>
+  <si>
+    <t>17-01-2023</t>
+  </si>
+  <si>
+    <t>18-01-2023</t>
+  </si>
+  <si>
+    <t>19-01-2023</t>
+  </si>
+  <si>
+    <t>20-01-2023</t>
+  </si>
+  <si>
+    <t>21-01-2023</t>
+  </si>
+  <si>
+    <t>22-01-2023</t>
+  </si>
+  <si>
+    <t>23-01-2023</t>
+  </si>
+  <si>
+    <t>24-01-2023</t>
+  </si>
+  <si>
+    <t>25-01-2023</t>
+  </si>
+  <si>
+    <t>26-01-2023</t>
+  </si>
+  <si>
+    <t>27-01-2023</t>
+  </si>
+  <si>
+    <t>28-01-2023</t>
+  </si>
+  <si>
+    <t>29-01-2023</t>
+  </si>
+  <si>
+    <t>30-01-2023</t>
+  </si>
+  <si>
+    <t>31-01-2023</t>
+  </si>
+  <si>
+    <t>01-02-2023</t>
+  </si>
+  <si>
+    <t>02-02-2023</t>
+  </si>
+  <si>
+    <t>03-02-2023</t>
+  </si>
+  <si>
+    <t>04-02-2023</t>
+  </si>
+  <si>
+    <t>05-02-2023</t>
+  </si>
+  <si>
+    <t>06-02-2023</t>
+  </si>
+  <si>
+    <t>07-02-2023</t>
+  </si>
+  <si>
+    <t>08-02-2023</t>
+  </si>
+  <si>
+    <t>09-02-2023</t>
+  </si>
+  <si>
+    <t>10-02-2023</t>
+  </si>
+  <si>
+    <t>11-02-2023</t>
+  </si>
+  <si>
+    <t>12-02-2023</t>
+  </si>
+  <si>
+    <t>13-02-2023</t>
+  </si>
+  <si>
+    <t>14-02-2023</t>
+  </si>
+  <si>
+    <t>15-02-2023</t>
+  </si>
+  <si>
+    <t>16-02-2023</t>
+  </si>
+  <si>
+    <t>17-02-2023</t>
+  </si>
+  <si>
+    <t>18-02-2023</t>
+  </si>
+  <si>
+    <t>19-02-2023</t>
+  </si>
+  <si>
+    <t>20-02-2023</t>
+  </si>
+  <si>
+    <t>21-02-2023</t>
+  </si>
+  <si>
+    <t>22-02-2023</t>
+  </si>
+  <si>
+    <t>23-02-2023</t>
+  </si>
+  <si>
+    <t>24-02-2023</t>
+  </si>
+  <si>
+    <t>25-02-2023</t>
+  </si>
+  <si>
+    <t>26-02-2023</t>
+  </si>
+  <si>
+    <t>27-02-2023</t>
+  </si>
+  <si>
+    <t>28-02-2023</t>
+  </si>
+  <si>
+    <t>01-03-2023</t>
+  </si>
+  <si>
+    <t>02-03-2023</t>
+  </si>
+  <si>
+    <t>03-03-2023</t>
+  </si>
+  <si>
+    <t>04-03-2023</t>
+  </si>
+  <si>
+    <t>05-03-2023</t>
+  </si>
+  <si>
+    <t>06-03-2023</t>
+  </si>
+  <si>
+    <t>07-03-2023</t>
+  </si>
+  <si>
+    <t>08-03-2023</t>
+  </si>
+  <si>
+    <t>09-03-2023</t>
+  </si>
+  <si>
+    <t>10-03-2023</t>
+  </si>
+  <si>
+    <t>11-03-2023</t>
+  </si>
+  <si>
+    <t>12-03-2023</t>
+  </si>
+  <si>
+    <t>13-03-2023</t>
+  </si>
+  <si>
+    <t>14-03-2023</t>
+  </si>
+  <si>
+    <t>15-03-2023</t>
+  </si>
+  <si>
+    <t>16-03-2023</t>
+  </si>
+  <si>
+    <t>17-03-2023</t>
+  </si>
+  <si>
+    <t>18-03-2023</t>
+  </si>
+  <si>
+    <t>19-03-2023</t>
+  </si>
+  <si>
+    <t>20-03-2023</t>
+  </si>
+  <si>
+    <t>21-03-2023</t>
+  </si>
+  <si>
+    <t>22-03-2023</t>
+  </si>
+  <si>
+    <t>23-03-2023</t>
+  </si>
+  <si>
+    <t>24-03-2023</t>
+  </si>
+  <si>
+    <t>25-03-2023</t>
+  </si>
+  <si>
+    <t>26-03-2023</t>
+  </si>
+  <si>
+    <t>27-03-2023</t>
+  </si>
+  <si>
+    <t>28-03-2023</t>
+  </si>
+  <si>
+    <t>29-03-2023</t>
+  </si>
+  <si>
+    <t>30-03-2023</t>
+  </si>
+  <si>
+    <t>31-03-2023</t>
+  </si>
+  <si>
+    <t>01-04-2023</t>
+  </si>
+  <si>
+    <t>02-04-2023</t>
+  </si>
+  <si>
+    <t>03-04-2023</t>
+  </si>
+  <si>
+    <t>04-04-2023</t>
+  </si>
+  <si>
+    <t>05-04-2023</t>
+  </si>
+  <si>
+    <t>06-04-2023</t>
+  </si>
+  <si>
+    <t>07-04-2023</t>
+  </si>
+  <si>
+    <t>08-04-2023</t>
+  </si>
+  <si>
+    <t>09-04-2023</t>
+  </si>
+  <si>
+    <t>10-04-2023</t>
+  </si>
+  <si>
+    <t>11-04-2023</t>
+  </si>
+  <si>
+    <t>12-04-2023</t>
+  </si>
+  <si>
+    <t>13-04-2023</t>
+  </si>
+  <si>
+    <t>14-04-2023</t>
+  </si>
+  <si>
+    <t>15-04-2023</t>
+  </si>
+  <si>
+    <t>16-04-2023</t>
+  </si>
+  <si>
+    <t>17-04-2023</t>
+  </si>
+  <si>
+    <t>18-04-2023</t>
+  </si>
+  <si>
+    <t>19-04-2023</t>
+  </si>
+  <si>
+    <t>20-04-2023</t>
+  </si>
+  <si>
+    <t>21-04-2023</t>
+  </si>
+  <si>
+    <t>22-04-2023</t>
+  </si>
+  <si>
+    <t>23-04-2023</t>
+  </si>
+  <si>
+    <t>24-04-2023</t>
+  </si>
+  <si>
+    <t>25-04-2023</t>
+  </si>
+  <si>
+    <t>26-04-2023</t>
+  </si>
+  <si>
+    <t>27-04-2023</t>
+  </si>
+  <si>
+    <t>28-04-2023</t>
+  </si>
+  <si>
+    <t>29-04-2023</t>
+  </si>
+  <si>
+    <t>30-04-2023</t>
+  </si>
+  <si>
+    <t>01-05-2023</t>
+  </si>
+  <si>
+    <t>02-05-2023</t>
+  </si>
+  <si>
+    <t>03-05-2023</t>
+  </si>
+  <si>
+    <t>04-05-2023</t>
+  </si>
+  <si>
+    <t>05-05-2023</t>
+  </si>
+  <si>
+    <t>06-05-2023</t>
+  </si>
+  <si>
+    <t>07-05-2023</t>
+  </si>
+  <si>
+    <t>08-05-2023</t>
+  </si>
+  <si>
+    <t>09-05-2023</t>
+  </si>
+  <si>
+    <t>10-05-2023</t>
+  </si>
+  <si>
+    <t>11-05-2023</t>
+  </si>
+  <si>
+    <t>12-05-2023</t>
+  </si>
+  <si>
+    <t>13-05-2023</t>
+  </si>
+  <si>
+    <t>14-05-2023</t>
+  </si>
+  <si>
+    <t>15-05-2023</t>
+  </si>
+  <si>
+    <t>16-05-2023</t>
+  </si>
+  <si>
+    <t>17-05-2023</t>
+  </si>
+  <si>
+    <t>18-05-2023</t>
+  </si>
+  <si>
+    <t>19-05-2023</t>
+  </si>
+  <si>
+    <t>20-05-2023</t>
+  </si>
+  <si>
+    <t>21-05-2023</t>
+  </si>
+  <si>
+    <t>22-05-2023</t>
+  </si>
+  <si>
+    <t>23-05-2023</t>
+  </si>
+  <si>
+    <t>24-05-2023</t>
+  </si>
+  <si>
+    <t>25-05-2023</t>
+  </si>
+  <si>
+    <t>26-05-2023</t>
+  </si>
+  <si>
+    <t>27-05-2023</t>
+  </si>
+  <si>
+    <t>28-05-2023</t>
+  </si>
+  <si>
+    <t>29-05-2023</t>
+  </si>
+  <si>
+    <t>30-05-2023</t>
+  </si>
+  <si>
+    <t>31-05-2023</t>
+  </si>
+  <si>
+    <t>01-06-2023</t>
+  </si>
+  <si>
+    <t>02-06-2023</t>
+  </si>
+  <si>
+    <t>03-06-2023</t>
+  </si>
+  <si>
+    <t>04-06-2023</t>
+  </si>
+  <si>
+    <t>05-06-2023</t>
+  </si>
+  <si>
+    <t>06-06-2023</t>
+  </si>
+  <si>
+    <t>07-06-2023</t>
+  </si>
+  <si>
+    <t>08-06-2023</t>
+  </si>
+  <si>
+    <t>09-06-2023</t>
+  </si>
+  <si>
+    <t>10-06-2023</t>
+  </si>
+  <si>
+    <t>11-06-2023</t>
+  </si>
+  <si>
+    <t>12-06-2023</t>
+  </si>
+  <si>
+    <t>13-06-2023</t>
+  </si>
+  <si>
+    <t>14-06-2023</t>
+  </si>
+  <si>
+    <t>15-06-2023</t>
+  </si>
+  <si>
+    <t>16-06-2023</t>
+  </si>
+  <si>
+    <t>17-06-2023</t>
+  </si>
+  <si>
+    <t>18-06-2023</t>
+  </si>
+  <si>
+    <t>19-06-2023</t>
+  </si>
+  <si>
+    <t>20-06-2023</t>
+  </si>
+  <si>
+    <t>21-06-2023</t>
+  </si>
+  <si>
+    <t>22-06-2023</t>
+  </si>
+  <si>
+    <t>23-06-2023</t>
+  </si>
+  <si>
+    <t>24-06-2023</t>
+  </si>
+  <si>
+    <t>25-06-2023</t>
+  </si>
+  <si>
+    <t>26-06-2023</t>
+  </si>
+  <si>
+    <t>27-06-2023</t>
+  </si>
+  <si>
+    <t>28-06-2023</t>
+  </si>
+  <si>
+    <t>29-06-2023</t>
+  </si>
+  <si>
+    <t>30-06-2023</t>
   </si>
 </sst>
 </file>
@@ -5866,10 +6409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1827"/>
+  <dimension ref="A1:B2008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1824" workbookViewId="0">
-      <selection activeCell="F1832" sqref="F1832"/>
+    <sheetView tabSelected="1" topLeftCell="A1996" workbookViewId="0">
+      <selection activeCell="B2013" sqref="B2013"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20493,6 +21036,1454 @@
         <v>99.080415806451612</v>
       </c>
     </row>
+    <row r="1828" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1828" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B1828">
+        <v>99.077029999999993</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1829" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B1829">
+        <v>99.074548709677416</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1830" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1830">
+        <v>99.072067419354838</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1831" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B1831">
+        <v>99.06958612903226</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1832" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B1832">
+        <v>99.067104838709668</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1833" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B1833">
+        <v>99.06462354838709</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1834" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B1834">
+        <v>99.062142258064512</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1835" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B1835">
+        <v>99.059660967741934</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1836" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B1836">
+        <v>99.057179677419356</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1837" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B1837">
+        <v>99.054698387096778</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1838" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B1838">
+        <v>99.052217096774186</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1839" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B1839">
+        <v>99.049735806451608</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1840" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1840">
+        <v>99.04725451612903</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1841" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B1841">
+        <v>99.044773225806452</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1842" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B1842">
+        <v>99.042291935483874</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1843" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B1843">
+        <v>99.039810645161296</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1844" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1844">
+        <v>99.037329354838704</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1845" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B1845">
+        <v>99.034848064516126</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1846" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B1846">
+        <v>99.032366774193548</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1847" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1847">
+        <v>99.02988548387097</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1848" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B1848">
+        <v>99.027404193548392</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1849" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B1849">
+        <v>99.024922903225814</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1850" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1850">
+        <v>99.022441612903222</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1851" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B1851">
+        <v>99.019960322580644</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1852" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B1852">
+        <v>99.017479032258066</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1853" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B1853">
+        <v>99.014997741935488</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1854" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B1854">
+        <v>99.01251645161291</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1855" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B1855">
+        <v>99.010035161290332</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1856" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B1856">
+        <v>99.00755387096774</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1857" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B1857">
+        <v>99.005072580645162</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1858" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B1858">
+        <v>99.002591290322584</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1859" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B1859">
+        <v>99.000110000000006</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1860" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B1860">
+        <v>98.998361428571428</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1861" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B1861">
+        <v>98.996612857142864</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1862" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1862">
+        <v>98.994864285714286</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1863" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B1863">
+        <v>98.993115714285722</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1864" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B1864">
+        <v>98.991367142857143</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1865" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B1865">
+        <v>98.989618571428579</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1866" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B1866">
+        <v>98.987870000000001</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1867" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B1867">
+        <v>98.986121428571437</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1868" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B1868">
+        <v>98.984372857142858</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1869" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B1869">
+        <v>98.982624285714294</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1870" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B1870">
+        <v>98.980875714285716</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1871" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B1871">
+        <v>98.979127142857152</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1872" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B1872">
+        <v>98.977378571428574</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1873" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B1873">
+        <v>98.975629999999995</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1874" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B1874">
+        <v>98.973881428571431</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1875" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B1875">
+        <v>98.972132857142853</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1876" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B1876">
+        <v>98.970384285714289</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1877" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B1877">
+        <v>98.96863571428571</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1878" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B1878">
+        <v>98.966887142857146</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1879" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B1879">
+        <v>98.965138571428568</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1880" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B1880">
+        <v>98.963390000000004</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1881" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B1881">
+        <v>98.961641428571426</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1882" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B1882">
+        <v>98.959892857142862</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1883" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B1883">
+        <v>98.958144285714283</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1884" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B1884">
+        <v>98.956395714285719</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1885" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B1885">
+        <v>98.954647142857141</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1886" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B1886">
+        <v>98.952898571428577</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1887" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B1887">
+        <v>98.951149999999998</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1888" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B1888">
+        <v>98.949947096774196</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1889" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B1889">
+        <v>98.948744193548379</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1890" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B1890">
+        <v>98.947541290322576</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1891" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B1891">
+        <v>98.946338387096773</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1892" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B1892">
+        <v>98.94513548387097</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1893" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B1893">
+        <v>98.943932580645154</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1894" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B1894">
+        <v>98.942729677419351</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1895" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B1895">
+        <v>98.941526774193548</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1896" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B1896">
+        <v>98.940323870967745</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1897" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B1897">
+        <v>98.939120967741928</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1898" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B1898">
+        <v>98.937918064516126</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1899" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B1899">
+        <v>98.936715161290323</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1900" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B1900">
+        <v>98.93551225806452</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1901" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B1901">
+        <v>98.934309354838703</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1902" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1902">
+        <v>98.9331064516129</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1903" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B1903">
+        <v>98.931903548387098</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1904" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B1904">
+        <v>98.930700645161295</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1905" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B1905">
+        <v>98.929497741935478</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1906" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B1906">
+        <v>98.928294838709675</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1907" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B1907">
+        <v>98.927091935483872</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1908" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B1908">
+        <v>98.92588903225807</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1909" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B1909">
+        <v>98.924686129032253</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1910" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B1910">
+        <v>98.92348322580645</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1911" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B1911">
+        <v>98.922280322580647</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1912" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B1912">
+        <v>98.921077419354845</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1913" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B1913">
+        <v>98.919874516129028</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1914" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B1914">
+        <v>98.918671612903225</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1915" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1915">
+        <v>98.917468709677422</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1916" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B1916">
+        <v>98.916265806451619</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1917" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B1917">
+        <v>98.915062903225802</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1918" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B1918">
+        <v>98.91386</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1919" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B1919">
+        <v>98.913551333333331</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1920" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B1920">
+        <v>98.913242666666662</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1921" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B1921">
+        <v>98.912934000000007</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1922" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B1922">
+        <v>98.912625333333338</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1923" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B1923">
+        <v>98.912316666666669</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1924" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B1924">
+        <v>98.912008</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1925" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B1925">
+        <v>98.911699333333331</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1926" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B1926">
+        <v>98.911390666666662</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1927" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B1927">
+        <v>98.911081999999993</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1928" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B1928">
+        <v>98.910773333333339</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1929" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B1929">
+        <v>98.91046466666667</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1930" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B1930">
+        <v>98.910156000000001</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1931" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B1931">
+        <v>98.909847333333332</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1932" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B1932">
+        <v>98.909538666666663</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1933" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B1933">
+        <v>98.909230000000008</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1934" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B1934">
+        <v>98.908921333333339</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1935" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B1935">
+        <v>98.90861266666667</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1936" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B1936">
+        <v>98.908304000000001</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1937" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B1937">
+        <v>98.907995333333332</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1938" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B1938">
+        <v>98.907686666666663</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1939" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B1939">
+        <v>98.907377999999994</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1940" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B1940">
+        <v>98.90706933333334</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1941" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B1941">
+        <v>98.906760666666671</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1942" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B1942">
+        <v>98.906452000000002</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1943" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B1943">
+        <v>98.906143333333333</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1944" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B1944">
+        <v>98.905834666666664</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1945" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1945">
+        <v>98.905526000000009</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1946" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B1946">
+        <v>98.90521733333334</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1947" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B1947">
+        <v>98.904908666666671</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1948" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B1948">
+        <v>98.904600000000002</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1949" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B1949">
+        <v>98.904044193548387</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1950" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B1950">
+        <v>98.903488387096772</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1951" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B1951">
+        <v>98.902932580645157</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1952" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B1952">
+        <v>98.902376774193556</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1953" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B1953">
+        <v>98.901820967741941</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1954" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B1954">
+        <v>98.901265161290326</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1955" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B1955">
+        <v>98.90070935483871</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1956" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B1956">
+        <v>98.900153548387095</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1957" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B1957">
+        <v>98.89959774193548</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1958" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B1958">
+        <v>98.899041935483879</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1959" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B1959">
+        <v>98.898486129032264</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1960" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B1960">
+        <v>98.897930322580649</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1961" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B1961">
+        <v>98.897374516129034</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1962" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B1962">
+        <v>98.896818709677419</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1963" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B1963">
+        <v>98.896262903225804</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1964" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B1964">
+        <v>98.895707096774203</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1965" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B1965">
+        <v>98.895151290322588</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1966" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B1966">
+        <v>98.894595483870972</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1967" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B1967">
+        <v>98.894039677419357</v>
+      </c>
+    </row>
+    <row r="1968" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1968" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B1968">
+        <v>98.893483870967742</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1969" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B1969">
+        <v>98.892928064516127</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1970" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B1970">
+        <v>98.892372258064526</v>
+      </c>
+    </row>
+    <row r="1971" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1971" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B1971">
+        <v>98.891816451612911</v>
+      </c>
+    </row>
+    <row r="1972" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1972" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B1972">
+        <v>98.891260645161296</v>
+      </c>
+    </row>
+    <row r="1973" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1973" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B1973">
+        <v>98.890704838709681</v>
+      </c>
+    </row>
+    <row r="1974" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1974" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B1974">
+        <v>98.890149032258066</v>
+      </c>
+    </row>
+    <row r="1975" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1975" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B1975">
+        <v>98.889593225806451</v>
+      </c>
+    </row>
+    <row r="1976" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1976" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B1976">
+        <v>98.88903741935485</v>
+      </c>
+    </row>
+    <row r="1977" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1977" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B1977">
+        <v>98.888481612903234</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1978" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B1978">
+        <v>98.887925806451619</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1979" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B1979">
+        <v>98.887370000000004</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1980" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B1980">
+        <v>98.886857666666671</v>
+      </c>
+    </row>
+    <row r="1981" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1981" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B1981">
+        <v>98.886345333333338</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1982" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B1982">
+        <v>98.885833000000005</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1983" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B1983">
+        <v>98.885320666666672</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1984" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B1984">
+        <v>98.884808333333339</v>
+      </c>
+    </row>
+    <row r="1985" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1985" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B1985">
+        <v>98.884296000000006</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1986" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B1986">
+        <v>98.883783666666673</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1987" t="s">
+        <v>1987</v>
+      </c>
+      <c r="B1987">
+        <v>98.88327133333334</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1988" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B1988">
+        <v>98.882759000000007</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1989" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B1989">
+        <v>98.882246666666674</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1990" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B1990">
+        <v>98.881734333333341</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1991" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B1991">
+        <v>98.881222000000008</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1992" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B1992">
+        <v>98.880709666666675</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1993" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B1993">
+        <v>98.880197333333342</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1994" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B1994">
+        <v>98.879684999999995</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1995" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B1995">
+        <v>98.879172666666662</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1996" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B1996">
+        <v>98.878660333333329</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1997" t="s">
+        <v>1997</v>
+      </c>
+      <c r="B1997">
+        <v>98.878147999999996</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1998" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B1998">
+        <v>98.877635666666663</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1999" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B1999">
+        <v>98.87712333333333</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2000" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2000">
+        <v>98.876610999999997</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2001" t="s">
+        <v>2001</v>
+      </c>
+      <c r="B2001">
+        <v>98.876098666666664</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2002" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B2002">
+        <v>98.875586333333331</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2003" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B2003">
+        <v>98.875073999999998</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2004" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B2004">
+        <v>98.874561666666665</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2005" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B2005">
+        <v>98.874049333333332</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2006" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B2006">
+        <v>98.873536999999999</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2007" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B2007">
+        <v>98.873024666666666</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2008" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B2008">
+        <v>98.872512333333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>